<commit_message>
Aggiunti alcuni grafici + consuntivo
</commit_message>
<xml_diff>
--- a/Piano di Progetto/Preventivo/AnalisiRequisiti.Economico.xlsx
+++ b/Piano di Progetto/Preventivo/AnalisiRequisiti.Economico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panoz\Documents\GitHub\Marvin\Piano di Progetto\Preventivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B630423-2039-478E-9097-A38997BDE6EE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E36D5-2793-47E5-9896-7D63EC8CF64C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{A9C5908B-2465-420D-9242-B7F005395B64}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Ruolo</t>
   </si>
@@ -255,6 +255,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-01D3-4673-871E-800908581F9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -272,6 +277,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-01D3-4673-871E-800908581F9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -289,6 +299,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-01D3-4673-871E-800908581F9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -306,6 +321,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-01D3-4673-871E-800908581F9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1326,7 +1346,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1376,8 +1396,8 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
+      <c r="C4" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,8 +1419,8 @@
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
+      <c r="C6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Preventivo finito + update
</commit_message>
<xml_diff>
--- a/Piano di Progetto/Preventivo/AnalisiRequisiti.Economico.xlsx
+++ b/Piano di Progetto/Preventivo/AnalisiRequisiti.Economico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panoz\Documents\GitHub\Marvin\Piano di Progetto\Preventivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39E36D5-2793-47E5-9896-7D63EC8CF64C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819D85D6-0616-4622-B1FC-8DB810BFA7A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{A9C5908B-2465-420D-9242-B7F005395B64}"/>
   </bookViews>
@@ -157,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +194,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,18 +399,18 @@
             <c:numRef>
               <c:f>(Foglio1!$C$2,Foglio1!$C$3,Foglio1!$C$5,Foglio1!$C$7)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
                   <c:v>720</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1650</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="General">
                   <c:v>840</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="3" formatCode="General">
                   <c:v>960</c:v>
                 </c:pt>
               </c:numCache>
@@ -1345,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1526DCFC-2621-45BC-859A-8A7F0D00817C}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,8 +1390,7 @@
       <c r="B3" s="3">
         <v>66</v>
       </c>
-      <c r="C3" s="3">
-        <f>25*B3</f>
+      <c r="C3" s="13">
         <v>1650</v>
       </c>
     </row>
@@ -1443,8 +1448,7 @@
         <f>SUM(B2:B7)</f>
         <v>196</v>
       </c>
-      <c r="C8" s="11">
-        <f>SUM(C2:C7)</f>
+      <c r="C8" s="14">
         <v>4170</v>
       </c>
     </row>

</xml_diff>